<commit_message>
One way Analysis of variance
</commit_message>
<xml_diff>
--- a/52/practice_data.xlsx
+++ b/52/practice_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Udemey\Data Analytics\50\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Udemey\Data Analytics\Git\52\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8265879-4DED-42F5-B12C-D971941016A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102302BC-9663-424F-B27F-9A71B641798A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2629820B-5075-0A45-8EC5-48C69810D758}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>Days Present</t>
   </si>
   <si>
-    <t>Accuracy of Work</t>
-  </si>
-  <si>
     <t>Meeting Project Deadlines</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
   </si>
   <si>
     <t>Sales Revenue Generated</t>
+  </si>
+  <si>
+    <t>Accuracy_of_Work</t>
   </si>
 </sst>
 </file>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B94492B4-EC22-B140-BC0B-C226297B5117}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -514,25 +514,25 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>22</v>
-      </c>
       <c r="K1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.4">
@@ -540,19 +540,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
       </c>
       <c r="D2">
         <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2">
         <v>85</v>
@@ -567,7 +567,7 @@
         <v>51638</v>
       </c>
       <c r="K2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.4">
@@ -575,19 +575,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
         <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
       </c>
       <c r="D3">
         <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G3">
         <v>90</v>
@@ -602,7 +602,7 @@
         <v>97797</v>
       </c>
       <c r="K3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.4">
@@ -610,19 +610,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4">
         <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G4">
         <v>80</v>
@@ -637,7 +637,7 @@
         <v>95341</v>
       </c>
       <c r="K4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
@@ -645,19 +645,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5">
         <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G5">
         <v>75</v>
@@ -672,7 +672,7 @@
         <v>91806</v>
       </c>
       <c r="K5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.4">
@@ -680,19 +680,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6">
         <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G6">
         <v>85</v>
@@ -707,7 +707,7 @@
         <v>64247</v>
       </c>
       <c r="K6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.4">
@@ -715,19 +715,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
         <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
       </c>
       <c r="D7">
         <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7">
         <v>95</v>
@@ -742,7 +742,7 @@
         <v>89988</v>
       </c>
       <c r="K7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.4">
@@ -750,19 +750,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
         <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
       </c>
       <c r="D8">
         <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G8">
         <v>70</v>
@@ -777,7 +777,7 @@
         <v>70934</v>
       </c>
       <c r="K8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.4">
@@ -785,19 +785,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9">
         <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G9">
         <v>80</v>
@@ -812,7 +812,7 @@
         <v>96578</v>
       </c>
       <c r="K9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.4">
@@ -820,19 +820,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10">
         <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G10">
         <v>90</v>
@@ -847,7 +847,7 @@
         <v>74219</v>
       </c>
       <c r="K10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.4">
@@ -855,19 +855,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11">
         <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G11">
         <v>85</v>
@@ -882,7 +882,7 @@
         <v>87009</v>
       </c>
       <c r="K11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.4">
@@ -890,19 +890,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
         <v>9</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
       </c>
       <c r="D12">
         <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G12">
         <v>75</v>
@@ -917,7 +917,7 @@
         <v>77785</v>
       </c>
       <c r="K12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.4">
@@ -925,19 +925,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="s">
         <v>14</v>
-      </c>
-      <c r="C13" t="s">
-        <v>15</v>
       </c>
       <c r="D13">
         <v>19</v>
       </c>
       <c r="E13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G13">
         <v>70</v>
@@ -952,7 +952,7 @@
         <v>97201</v>
       </c>
       <c r="K13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.4">
@@ -960,19 +960,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14">
         <v>23</v>
       </c>
       <c r="E14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G14">
         <v>80</v>
@@ -987,7 +987,7 @@
         <v>67730</v>
       </c>
       <c r="K14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.4">
@@ -995,19 +995,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15">
         <v>21</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G15">
         <v>90</v>
@@ -1022,7 +1022,7 @@
         <v>93427</v>
       </c>
       <c r="K15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.4">
@@ -1030,19 +1030,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16">
         <v>24</v>
       </c>
       <c r="E16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G16">
         <v>65</v>
@@ -1057,7 +1057,7 @@
         <v>77172</v>
       </c>
       <c r="K16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.4">
@@ -1065,19 +1065,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
         <v>9</v>
-      </c>
-      <c r="C17" t="s">
-        <v>10</v>
       </c>
       <c r="D17">
         <v>18</v>
       </c>
       <c r="E17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G17">
         <v>75</v>
@@ -1092,7 +1092,7 @@
         <v>85737</v>
       </c>
       <c r="K17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.4">
@@ -1100,19 +1100,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
         <v>14</v>
-      </c>
-      <c r="C18" t="s">
-        <v>15</v>
       </c>
       <c r="D18">
         <v>20</v>
       </c>
       <c r="E18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G18">
         <v>85</v>
@@ -1127,7 +1127,7 @@
         <v>74871</v>
       </c>
       <c r="K18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.4">
@@ -1135,19 +1135,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19">
         <v>22</v>
       </c>
       <c r="E19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G19">
         <v>80</v>
@@ -1162,7 +1162,7 @@
         <v>63245</v>
       </c>
       <c r="K19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.4">
@@ -1170,19 +1170,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D20">
         <v>25</v>
       </c>
       <c r="E20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G20">
         <v>70</v>
@@ -1197,7 +1197,7 @@
         <v>53169</v>
       </c>
       <c r="K20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.4">
@@ -1205,19 +1205,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21">
         <v>19</v>
       </c>
       <c r="E21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G21">
         <v>65</v>
@@ -1232,7 +1232,7 @@
         <v>81770</v>
       </c>
       <c r="K21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.4">
@@ -1240,19 +1240,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" t="s">
         <v>9</v>
-      </c>
-      <c r="C22" t="s">
-        <v>10</v>
       </c>
       <c r="D22">
         <v>23</v>
       </c>
       <c r="E22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G22">
         <v>75</v>
@@ -1267,7 +1267,7 @@
         <v>78482</v>
       </c>
       <c r="K22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.4">
@@ -1275,19 +1275,19 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" t="s">
         <v>14</v>
-      </c>
-      <c r="C23" t="s">
-        <v>15</v>
       </c>
       <c r="D23">
         <v>21</v>
       </c>
       <c r="E23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G23">
         <v>85</v>
@@ -1302,7 +1302,7 @@
         <v>57836</v>
       </c>
       <c r="K23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.4">
@@ -1310,19 +1310,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D24">
         <v>24</v>
       </c>
       <c r="E24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G24">
         <v>60</v>
@@ -1337,7 +1337,7 @@
         <v>62885</v>
       </c>
       <c r="K24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.4">
@@ -1345,19 +1345,19 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D25">
         <v>18</v>
       </c>
       <c r="E25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G25">
         <v>70</v>
@@ -1372,7 +1372,7 @@
         <v>52579</v>
       </c>
       <c r="K25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.4">
@@ -1380,19 +1380,19 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D26">
         <v>20</v>
       </c>
       <c r="E26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G26">
         <v>80</v>
@@ -1407,7 +1407,7 @@
         <v>75795</v>
       </c>
       <c r="K26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.4">
@@ -1415,19 +1415,19 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D27">
         <v>19</v>
       </c>
       <c r="E27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G27">
         <v>65</v>
@@ -1442,7 +1442,7 @@
         <v>81770</v>
       </c>
       <c r="K27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.4">
@@ -1450,19 +1450,19 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" t="s">
         <v>9</v>
-      </c>
-      <c r="C28" t="s">
-        <v>10</v>
       </c>
       <c r="D28">
         <v>23</v>
       </c>
       <c r="E28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G28">
         <v>75</v>
@@ -1477,7 +1477,7 @@
         <v>78482</v>
       </c>
       <c r="K28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.4">
@@ -1485,19 +1485,19 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
         <v>14</v>
-      </c>
-      <c r="C29" t="s">
-        <v>15</v>
       </c>
       <c r="D29">
         <v>21</v>
       </c>
       <c r="E29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G29">
         <v>85</v>
@@ -1512,7 +1512,7 @@
         <v>57836</v>
       </c>
       <c r="K29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.4">
@@ -1520,19 +1520,19 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D30">
         <v>24</v>
       </c>
       <c r="E30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G30">
         <v>60</v>
@@ -1547,7 +1547,7 @@
         <v>62885</v>
       </c>
       <c r="K30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.4">
@@ -1555,19 +1555,19 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D31">
         <v>18</v>
       </c>
       <c r="E31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G31">
         <v>70</v>
@@ -1582,7 +1582,7 @@
         <v>52579</v>
       </c>
       <c r="K31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.4">
@@ -1590,19 +1590,19 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D32">
         <v>20</v>
       </c>
       <c r="E32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G32">
         <v>80</v>
@@ -1617,7 +1617,7 @@
         <v>75795</v>
       </c>
       <c r="K32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>